<commit_message>
Modified HomePageTest.xlsx file it the physical folder.
</commit_message>
<xml_diff>
--- a/InputData/HomePageTest.xlsx
+++ b/InputData/HomePageTest.xlsx
@@ -4,13 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8235" windowHeight="7455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18045" windowHeight="4800"/>
   </bookViews>
   <sheets>
     <sheet name="Keyword" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -432,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,7 +473,6 @@
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -527,9 +525,6 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Modified readObectAndPerformOpertions method and wrote description of testLogout method.
</commit_message>
<xml_diff>
--- a/InputData/HomePageTest.xlsx
+++ b/InputData/HomePageTest.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Keyword</t>
   </si>
@@ -67,6 +67,18 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>welcome</t>
+  </si>
+  <si>
+    <t>logout</t>
+  </si>
+  <si>
+    <t>css</t>
   </si>
 </sst>
 </file>
@@ -123,10 +135,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,7 +444,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -525,8 +538,37 @@
       </c>
       <c r="E6" s="2"/>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added new test method, testEmployeeSearch in class, HomePageTest.java
</commit_message>
<xml_diff>
--- a/InputData/HomePageTest.xlsx
+++ b/InputData/HomePageTest.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>Keyword</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>css</t>
+  </si>
+  <si>
+    <t>EmpoyeeSearch</t>
+  </si>
+  <si>
+    <t>employeename</t>
+  </si>
+  <si>
+    <t>search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a </t>
   </si>
 </sst>
 </file>
@@ -444,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,6 +578,49 @@
       </c>
       <c r="E8" s="2"/>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Made excel reader a generic method.
</commit_message>
<xml_diff>
--- a/InputData/HomePageTest.xlsx
+++ b/InputData/HomePageTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="100" windowWidth="14800" windowHeight="7660"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14000"/>
   </bookViews>
   <sheets>
     <sheet name="Keyword" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="18">
   <si>
     <t>Keyword</t>
   </si>
@@ -67,16 +67,45 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>logout</t>
+  </si>
+  <si>
+    <t>signin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -96,7 +125,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -119,16 +148,89 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -431,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -446,7 +548,7 @@
     <col min="5" max="5" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -463,7 +565,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -472,8 +574,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="2"/>
+    <row r="3" spans="1:6">
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -483,7 +584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -498,7 +599,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -513,7 +614,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>9</v>
@@ -525,6 +626,111 @@
         <v>15</v>
       </c>
       <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="B10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="B12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Re-factored and used the following methods,  testEmployeeSearch() and testLogout(). And also made changes in HomePageTest.xlsx and object.properties
</commit_message>
<xml_diff>
--- a/InputData/HomePageTest.xlsx
+++ b/InputData/HomePageTest.xlsx
@@ -10,7 +10,6 @@
     <sheet name="Keyword" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>Keyword</t>
   </si>
@@ -70,7 +69,28 @@
     <t>id</t>
   </si>
   <si>
+    <t>SearchEmployee</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>employeeName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a </t>
+  </si>
+  <si>
+    <t>searchButton</t>
+  </si>
+  <si>
+    <t>welcome</t>
+  </si>
+  <si>
     <t>logout</t>
+  </si>
+  <si>
+    <t>css</t>
   </si>
 </sst>
 </file>
@@ -123,7 +143,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -147,51 +167,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -208,15 +189,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -287,7 +266,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -322,7 +301,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -531,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,61 +603,86 @@
         <v>15</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+      <c r="B10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="C11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="E11" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25"/>
+      <c r="E12" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>